<commit_message>
added a script to execute ssr analysis and merge with the main script
</commit_message>
<xml_diff>
--- a/src/outputs/1-data_fao_groups.xlsx
+++ b/src/outputs/1-data_fao_groups.xlsx
@@ -379,12 +379,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Y2013_645</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Y2013_664</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Y2013_645</t>
         </is>
       </c>
     </row>

</xml_diff>